<commit_message>
Add microplate layout read implementation
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -926,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>